<commit_message>
feature/batch run and update log
</commit_message>
<xml_diff>
--- a/model_runs.xlsx
+++ b/model_runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/valuation-model-UI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B49376-02BB-5544-95BA-97D7E68E0868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4B7D5C-F4B7-9A40-AC3E-052FBA2DAC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12240" yWindow="-15600" windowWidth="26540" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18180" yWindow="-23180" windowWidth="32280" windowHeight="22020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>run_number</t>
   </si>
@@ -49,22 +49,58 @@
     <t>product_groups</t>
   </si>
   <si>
-    <t>Business%20Development%20and%20Thought%20Leadership/Valuation%20Model%20Development/Run1/Assumptions/Assumptions.xlsx</t>
-  </si>
-  <si>
-    <t>Business%20Development%20and%20Thought%20Leadership/Valuation%20Model%20Development/Run1/model%20point%20files</t>
-  </si>
-  <si>
-    <t>Business%20Development%20and%20Thought%20Leadership/Valuation%20Model%20Development/Run1/outputs</t>
-  </si>
-  <si>
     <t>Model Points.xlsx</t>
   </si>
   <si>
-    <t>Term_Model_v0.4</t>
-  </si>
-  <si>
-    <t>https://datalyactuarial.sharepoint.com/sites/DatalyActuarial/Shared%20Documents/Business%20Development%20and%20Thought%20Leadership/Valuation%20Model%20Development/Run1/models</t>
+    <t>Basic_Term_Model_v0.4wRPG</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Opening</t>
+  </si>
+  <si>
+    <t>Projection period from 30 to 20</t>
+  </si>
+  <si>
+    <t>valiadation date change to end of 2024</t>
+  </si>
+  <si>
+    <t>Business%20Development%20and%20Thought%20Leadership/Valuation%20Model%20Development/demo/Run1/outputs</t>
+  </si>
+  <si>
+    <t>Business%20Development%20and%20Thought%20Leadership/Valuation%20Model%20Development/demo/Run2/outputs</t>
+  </si>
+  <si>
+    <t>Business%20Development%20and%20Thought%20Leadership/Valuation%20Model%20Development/demo/Run3/outputs</t>
+  </si>
+  <si>
+    <t>Business%20Development%20and%20Thought%20Leadership/Valuation%20Model%20Development/demo/Run1/model%20point%20files</t>
+  </si>
+  <si>
+    <t>Business%20Development%20and%20Thought%20Leadership/Valuation%20Model%20Development/demo/Run2/model%20point%20files</t>
+  </si>
+  <si>
+    <t>Business%20Development%20and%20Thought%20Leadership/Valuation%20Model%20Development/demo/Run3/model%20point%20files</t>
+  </si>
+  <si>
+    <t>https://datalyactuarial.sharepoint.com/sites/DatalyActuarial/Shared%20Documents/Business%20Development%20and%20Thought%20Leadership/Valuation%20Model%20Development/demo/Run2/models</t>
+  </si>
+  <si>
+    <t>https://datalyactuarial.sharepoint.com/sites/DatalyActuarial/Shared%20Documents/Business%20Development%20and%20Thought%20Leadership/Valuation%20Model%20Development/demo/Run3/models</t>
+  </si>
+  <si>
+    <t>https://datalyactuarial.sharepoint.com/sites/DatalyActuarial/Shared%20Documents/Business%20Development%20and%20Thought%20Leadership/Valuation%20Model%20Development/demo/Run1/models</t>
+  </si>
+  <si>
+    <t>Business%20Development%20and%20Thought%20Leadership/Valuation%20Model%20Development/demo/Run1/Assumptions/Assumptions.xlsx</t>
+  </si>
+  <si>
+    <t>Business%20Development%20and%20Thought%20Leadership/Valuation%20Model%20Development/demo/Run2/Assumptions/Assumptions.xlsx</t>
+  </si>
+  <si>
+    <t>Business%20Development%20and%20Thought%20Leadership/Valuation%20Model%20Development/demo/Run3/Assumptions/Assumptions.xlsx</t>
   </si>
 </sst>
 </file>
@@ -478,115 +514,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="109.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="158" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="105" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="91.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.1640625" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2">
+        <v>30</v>
+      </c>
+      <c r="H2" s="3">
+        <v>45473</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2">
-        <v>30</v>
-      </c>
-      <c r="G2" s="3">
-        <v>45292</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3" s="3">
+        <v>45473</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4" s="3">
+        <v>45657</v>
+      </c>
+      <c r="I4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3">
-        <v>25</v>
-      </c>
-      <c r="G3" s="3">
-        <v>45444</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
+      <c r="J4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{CDC68A26-08A5-DF41-AFE2-D65D59B36E36}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{CDC68A26-08A5-DF41-AFE2-D65D59B36E36}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{5DE44A01-B0D8-2141-9467-26F0FE99D117}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{63891164-4445-A74D-B53F-703DE7166903}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>